<commit_message>
JSON'dan Excel'e dönüştürme işlevselliği için bir GUI eklendi. Hata yönetimi ve kullanıcı bildirimleri geliştirildi. README dosyasında GUI kullanımı ve güncellemeler yapıldı.
</commit_message>
<xml_diff>
--- a/output/converted.xlsx
+++ b/output/converted.xlsx
@@ -14,24 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>Ayşe</t>
-  </si>
-  <si>
-    <t>Mehmet</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>op</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>assets</t>
+  </si>
+  <si>
+    <t>fonts</t>
+  </si>
+  <si>
+    <t>layers</t>
+  </si>
+  <si>
+    <t>markers</t>
+  </si>
+  <si>
+    <t>props</t>
+  </si>
+  <si>
+    <t>chars</t>
+  </si>
+  <si>
+    <t>5.12.1</t>
+  </si>
+  <si>
+    <t>Comp 2</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>{'list': [{'fName': 'Pacifico-Regular', 'fFamily': 'Pacifico', 'fStyle': 'Regular', 'ascent': 94.498718297109}]}</t>
+  </si>
+  <si>
+    <t>[{'ddd': 0, 'ind': 1, 'ty': 5, 'nm': 'SAYFA BULUNAMADI', 'sr': 1, 'ks': {'o': {'a': 0, 'k': 100, 'ix': 11}, 'r': {'a': 0, 'k': 0, 'ix': 10}, 'p': {'a': 1, 'k': [{'i': {'x': 0.833, 'y': 0.833}, 'o': {'x': 0.167, 'y': 0.167}, 't': 0, 's': [-208, 558.286, 0], 'to': [0, 0, 0], 'ti': [0, 0, 0]}, {'i': {'x': 0.833, 'y': 0.833}, 'o': {'x': 0.167, 'y': 0.167}, 't': 11, 's': [11.429, 658.857, 0], 'to': [0, 0, 0], 'ti': [0, 0, 0]}, {'i': {'x': 0.833, 'y': 0.833}, 'o': {'x': 0.167, 'y': 0.167}, 't': 21, 's': [280, 773.143, 0], 'to': [0, 0, 0], 'ti': [0, 0, 0]}, {'t': 29.0000011811942, 's': [753.143, 956, 0]}], 'ix': 2, 'l': 2}, 'a': {'a': 0, 'k': [0, 0, 0], 'ix': 1, 'l': 2}, 's': {'a': 0, 'k': [100, 100, 100], 'ix': 6, 'l': 2}}, 'ao': 0, 'ef': [{'ty': 29, 'nm': 'Gaussian Blur', 'np': 5, 'mn': 'ADBE Gaussian Blur 2', 'ix': 1, 'en': 1, 'ef': [{'ty': 0, 'nm': 'Blurriness', 'mn': 'ADBE Gaussian Blur 2-0001', 'ix': 1, 'v': {'a': 0, 'k': 0, 'ix': 1}}, {'ty': 7, 'nm': 'Blur Dimensions', 'mn': 'ADBE Gaussian Blur 2-0002', 'ix': 2, 'v': {'a': 0, 'k': 1, 'ix': 2}}, {'ty': 7, 'nm': 'Repeat Edge Pixels', 'mn': 'ADBE Gaussian Blur 2-0003', 'ix': 3, 'v': {'a': 0, 'k': 1, 'ix': 3}}]}], 't': {'d': {'k': [{'s': {'sz': [619.428588867188, 170.285720825195], 'ps': [-309.714294433594, -85.1428604125977], 's': 30, 'f': 'Pacifico-Regular', 't': 'SAYFA BULUNAMADI', 'ca': 0, 'j': 2, 'tr': 0, 'lh': 36, 'ls': 0, 'fc': [0.922, 0.922, 0.922]}, 't': 0}]}, 'p': {}, 'm': {'g': 1, 'a': {'a': 0, 'k': [0, 0], 'ix': 2}}, 'a': []}, 'ip': 0, 'op': 900.000036657751, 'st': 0, 'ct': 1, 'bm': 0}, {'ddd': 0, 'ind': 2, 'ty': 5, 'nm': '404', 'sr': 1, 'ks': {'o': {'a': 0, 'k': 100, 'ix': 11}, 'r': {'a': 0, 'k': 0, 'ix': 10}, 'p': {'a': 1, 'k': [{'i': {'x': 0.833, 'y': 0.833}, 'o': {'x': 0.167, 'y': 0.167}, 't': 0, 's': [-269.143, 432, 0], 'to': [0, 0, 0], 'ti': [0, 0, 0]}, {'i': {'x': 0.833, 'y': 0.833}, 'o': {'x': 0.167, 'y': 0.167}, 't': 11, 's': [-10.857, 524.571, 0], 'to': [0, 0, 0], 'ti': [0, 0, 0]}, {'i': {'x': 0.833, 'y': 0.833}, 'o': {'x': 0.167, 'y': 0.167}, 't': 21, 's': [284, 628.571, 0], 'to': [0, 0, 0], 'ti': [0, 0, 0]}, {'t': 29.0000011811942, 's': [748, 788.571, 0]}], 'ix': 2, 'l': 2}, 'a': {'a': 0, 'k': [0, 0, 0], 'ix': 1, 'l': 2}, 's': {'a': 0, 'k': [100, 100, 100], 'ix': 6, 'l': 2}}, 'ao': 0, 'ef': [{'ty': 29, 'nm': 'Gaussian Blur', 'np': 5, 'mn': 'ADBE Gaussian Blur 2', 'ix': 1, 'en': 1, 'ef': [{'ty': 0, 'nm': 'Blurriness', 'mn': 'ADBE Gaussian Blur 2-0001', 'ix': 1, 'v': {'a': 0, 'k': 0, 'ix': 1}}, {'ty': 7, 'nm': 'Blur Dimensions', 'mn': 'ADBE Gaussian Blur 2-0002', 'ix': 2, 'v': {'a': 0, 'k': 1, 'ix': 2}}, {'ty': 7, 'nm': 'Repeat Edge Pixels', 'mn': 'ADBE Gaussian Blur 2-0003', 'ix': 3, 'v': {'a': 0, 'k': 1, 'ix': 3}}]}], 't': {'d': {'k': [{'s': {'sz': [977.142883300781, 512], 'ps': [-488.571441650391, -256], 's': 300, 'f': 'Pacifico-Regular', 't': '404', 'ca': 0, 'j': 2, 'tr': 0, 'lh': 360, 'ls': 0, 'fc': [0.922, 0.922, 0.922]}, 't': 0}]}, 'p': {}, 'm': {'g': 1, 'a': {'a': 0, 'k': [0, 0], 'ix': 2}}, 'a': []}, 'ip': 0, 'op': 900.000036657751, 'st': 0, 'ct': 1, 'bm': 0}]</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>[{'ch': '4', 'size': 300, 'style': 'Regular', 'w': 57.7, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[3.533, 0], [0, 0], [-1.2, 5.667], [0, 0.867], [3.4, 0], [1.2, -1.1], [0.533, -2.066], [0.8, -6.2], [0, 0], [-6.534, 11.934], [0, 1.134], [0.766, 0.667], [1.466, 0], [1.3, -0.966], [1.266, -2.333], [2.933, -8.533], [0, -1.266], [-1.134, -1.333], [-1.467, 0], [-9.667, 0], [0, 0], [0, -0.733], [-3.534, 0], [-1.1, 1.066], [-0.2, 3.067], [0, 0], [0, 0], [-1.334, 0.934], [0, 2.4]], 'o': [[0, 0], [0.933, -6.133], [0.133, -0.466], [0, -2.933], [-2.134, 0], [-1.2, 1.1], [-1.4, 5.6], [0, 0], [2.666, -7.333], [0.666, -1.133], [0, -1.066], [-0.767, -0.666], [-2.734, 0], [-1.3, 0.967], [-5.867, 10.867], [-0.467, 1.4], [0, 2.134], [1.133, 1.334], [5, 0.067], [0, 0], [-0.067, 0.4], [0, 4.334], [2.466, 0], [1.1, -1.066], [0, 0], [0, 0], [2.866, 0], [1.333, -0.933], [0, -3]], 'v': [[49.9, -22.5], [46.3, -22.5], [49.5, -40.2], [49.7, -42.2], [44.6, -46.6], [39.6, -44.95], [37, -40.2], [33.7, -22.5], [18.3, -22.5], [32.1, -51.4], [33.1, -54.8], [31.95, -57.4], [28.6, -58.4], [22.55, -56.95], [18.7, -52], [5.5, -22.9], [4.8, -18.9], [6.5, -13.7], [10.4, -11.7], [32.4, -11.6], [31.9, -6.7], [31.8, -5], [37.1, 1.5], [42.45, -0.1], [44.4, -6.3], [44.8, -11.6], [46.9, -11.6], [53.2, -13], [55.2, -18]], 'c': True}, 'ix': 2}, 'nm': '4', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': '4', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': '0', 'size': 300, 'style': 'Regular', 'w': 54.3, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[-6.534, 0], [-3.767, 2.867], [-2.1, 5.167], [0, 6.734], [3.566, 4.267], [6.533, 0], [3.766, -2.866], [2.1, -5.166], [0, -6.733], [-3.567, -4.266]], 'o': [[5, 0], [3.766, -2.866], [2.1, -5.166], [0, -7.933], [-3.567, -4.266], [-5, 0], [-3.767, 2.867], [-2.1, 5.167], [0, 7.934], [3.566, 4.267]], 'v': [[25.6, 0.5], [38.75, -3.8], [47.55, -15.85], [50.7, -33.7], [45.35, -52], [30.2, -58.4], [17.05, -54.1], [8.25, -42.05], [5.1, -24.2], [10.45, -5.9]], 'c': True}, 'ix': 2}, 'nm': '0', 'mn': 'ADBE Vector Shape - Group', 'hd': False}, {'ind': 1, 'ty': 'sh', 'ix': 2, 'ks': {'a': 0, 'k': {'i': [[3.6, 0], [1.5, 2.4], [0, 4.6], [-2.067, 4.034], [-3.6, 0], [-1.534, -2.433], [0, -4.6], [2.066, -4]], 'o': [[-3, 0], [-1.5, -2.4], [0, -6.866], [2.066, -4.033], [2.933, 0], [1.533, 2.434], [0, 6.867], [-2.067, 4]], 'v': [[26.6, -10.7], [19.85, -14.3], [17.6, -24.8], [20.7, -41.15], [29.2, -47.2], [35.9, -43.55], [38.2, -33], [35.1, -16.7]], 'c': True}, 'ix': 2}, 'nm': '0', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': '0', 'np': 5, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'S', 'size': 30, 'style': 'Regular', 'w': 69.3, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[-8.867, 0], [-5.967, 4.234], [0, 7.867], [2.166, 2.867], [3.066, 1.667], [5.066, 2.067], [2.333, 1.2], [1.566, 1.8], [0, 2.534], [-3.034, 2.1], [-5.734, 0], [-2.734, -1.466], [0, -2.8], [0.2, -2], [0, -1.266], [-1.167, -1.066], [-1.734, 0], [-1.267, 2.134], [0, 4.2], [2.433, 2.934], [4.066, 1.434], [4.866, 0], [4.833, -2.066], [2.566, -3.733], [0, -4.8], [-2.3, -3.1], [-3.234, -1.8], [-5.134, -2], [-2.2, -1.1], [-1.467, -1.633], [0, -2.266], [3.2, -2.033], [5.666, 0], [3.033, 1.467], [0, 3], [-0.1, 0.667], [0, 0.267], [0, 1.334], [1.133, 0.934], [1.8, 0], [1.266, -1.933], [0, -3.666], [-5.334, -3.366]], 'o': [[10, 0], [5.966, -4.233], [0, -4.2], [-2.167, -2.866], [-3.067, -1.666], [-4.2, -1.666], [-2.334, -1.2], [-1.567, -1.8], [0, -3.8], [3.033, -2.1], [4.066, 0], [2.733, 1.467], [0, 0.534], [-0.2, 1.067], [0, 1.467], [1.166, 1.067], [2.466, 0], [1.266, -2.133], [0, -4.266], [-2.434, -2.933], [-4.067, -1.433], [-6.534, 0], [-4.834, 2.067], [-2.567, 3.734], [0, 4.6], [2.3, 3.1], [3.233, 1.8], [4, 1.6], [2.2, 1.1], [1.466, 1.634], [0, 3.667], [-3.2, 2.034], [-5.467, 0], [-3.034, -1.466], [0, -0.733], [0.1, -0.666], [0.2, -1], [0, -1.466], [-1.134, -0.933], [-2.467, 0], [-1.267, 1.934], [0, 6.934], [5.333, 3.367]], 'v': [[32.7, 0.8], [56.65, -5.55], [65.6, -23.7], [62.35, -34.3], [54.5, -41.1], [42.3, -46.7], [32.5, -51], [26.65, -55.5], [24.3, -62], [28.85, -70.85], [42, -74], [52.2, -71.8], [56.3, -65.4], [56, -61.6], [55.7, -58.1], [57.45, -54.3], [61.8, -52.7], [67.4, -55.9], [69.3, -65.4], [65.65, -76.2], [55.9, -82.75], [42.5, -84.9], [25.45, -81.8], [14.35, -73.1], [10.5, -60.3], [13.95, -48.75], [22.25, -41.4], [34.8, -35.7], [44.1, -31.65], [49.6, -27.55], [51.8, -21.7], [47, -13.15], [33.7, -10.1], [20.95, -12.3], [16.4, -19], [16.55, -21.1], [16.7, -22.5], [17, -26], [15.3, -29.6], [10.9, -31], [5.3, -28.1], [3.4, -19.7], [11.4, -4.25]], 'c': True}, 'ix': 2}, 'nm': 'S', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'S', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'A', 'size': 30, 'style': 'Regular', 'w': 78.6, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[-4.6, 0], [-4.934, 10.334], [-2.867, -2.7], [-4.667, 0], [-3.134, 2.067], [-3.267, 3.934], [0, 2.6], [0.5, 0.8], [0.866, 0], [0.8, -0.933], [1.933, -1.433], [2.133, 0], [1.066, 1.634], [0, 3.6], [-1.434, 7.834], [-1.734, 6.467], [0, 0.534], [4.733, 0], [1.2, -0.666], [0.4, -1.866], [2.533, -7.466], [3.066, -3.333], [4.066, 0], [2.233, 3.1], [0, 5.667], [-2.934, 6.734], [-5.934, 4.1], [-8.467, 0], [-2.467, -0.366], [-3.467, -0.8], [-0.534, 0], [-1.3, 1.534], [0, 1.734], [1.866, 0.534], [3.5, 0.467], [3.066, 0], [8.466, -5.233], [4.333, -8.633], [0, -10.133], [-2.134, -4.3], [-3.7, -2.266]], 'o': [[9.6, 0], [0.733, 4.934], [2.866, 2.7], [4.533, 0], [3.133, -2.066], [1.266, -1.533], [0, -1.4], [-0.5, -0.8], [-1, 0], [-2.934, 3.467], [-1.934, 1.434], [-2.2, 0], [-1.067, -1.633], [0, -4.066], [1.433, -7.833], [0.2, -0.8], [0, -3.066], [-2, 0], [-1.2, 0.667], [-2.467, 12.8], [-2.534, 7.467], [-3.067, 3.334], [-3.6, 0], [-2.234, -3.1], [0, -7.8], [2.933, -6.733], [5.933, -4.1], [2.733, 0], [2.466, 0.367], [0.266, 0.067], [1.733, 0], [1.3, -1.533], [0, -2.133], [-2.867, -0.933], [-3.5, -0.466], [-11.867, 0], [-8.467, 5.234], [-4.334, 8.634], [0, 5.867], [2.133, 4.3], [3.7, 2.267]], 'v': [[30, 0.5], [51.8, -15], [57.2, -3.55], [68.5, 0.5], [80, -2.6], [89.6, -11.6], [91.5, -17.8], [90.75, -21.1], [88.7, -22.3], [86, -20.9], [78.7, -13.55], [72.6, -11.4], [67.7, -13.85], [66.1, -21.7], [68.25, -39.55], [73, -61], [73.3, -63], [66.2, -67.6], [61.4, -66.6], [59, -62.8], [51.5, -32.4], [43.1, -16.2], [32.4, -11.2], [23.65, -15.85], [20.3, -29], [24.7, -50.8], [38, -67.05], [59.6, -73.2], [67.4, -72.65], [76.3, -70.9], [77.5, -70.8], [82.05, -73.1], [84, -78], [81.2, -82], [71.65, -84.1], [61.8, -84.8], [31.3, -76.95], [12.1, -56.15], [5.6, -28], [8.8, -12.75], [17.55, -2.9]], 'c': True}, 'ix': 2}, 'nm': 'A', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'A', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'Y', 'size': 30, 'style': 'Regular', 'w': 85.1, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[0.4, -0.133], [4.866, -1.333], [-0.767, 5.067], [-0.667, 4.8], [-1.4, 9.934], [0, 0.8], [4.666, 0], [1.2, -1.233], [0.333, -2.933], [3.033, -8.066], [3.766, -3.966], [3.6, 0], [1.2, 1.467], [0, 3.4], [-0.4, 2.034], [-0.8, 3.334], [-0.634, 3.634], [0, 3.467], [2.3, 2.467], [4.066, 0], [6.8, -9.333], [0, -2.066], [-0.7, -0.9], [-0.934, 0], [-0.934, 1.267], [-2.634, 1.9], [-1.934, 0], [0, -3.2], [0.5, -2.733], [1, -4.6], [0.533, -2.966], [0, -2.466], [-3, -3.5], [-5.734, 0], [-4.867, 4.067], [-3.134, 8.267], [0.266, -1.6], [0, 0], [6.266, -5.466], [0, -7], [-3.034, -2.7], [-5.534, 0], [-5.567, 6.3], [-1.867, 13.133], [0, 0], [-6.067, 1.134], [-0.7, 1.1], [0, 1.6], [2.266, 0]], 'o': [[-5.4, 1.067], [0.733, -5.2], [0.766, -5.066], [1.2, -8], [0.066, -0.466], [0, -4.666], [-2.267, 0], [-1.2, 1.234], [-1.334, 11.667], [-3.034, 8.067], [-3.767, 3.967], [-3, 0], [-1.2, -1.466], [0, -1.333], [0.4, -2.033], [1.266, -5.6], [0.633, -3.633], [0, -4.8], [-2.3, -2.466], [-9.134, 0], [-1.867, 2.6], [0, 1.134], [0.7, 0.9], [1.133, 0], [2.933, -3.933], [2.633, -1.9], [2.466, 0], [0, 2.134], [-0.5, 2.734], [-1.134, 5.067], [-0.534, 2.967], [0, 5.534], [3, 3.5], [6, 0], [4.866, -4.066], [-0.4, 2.667], [0, 0], [-12.734, 4.2], [-6.267, 5.466], [0, 4.2], [3.033, 2.7], [8.333, 0], [5.566, -6.3], [0, 0], [5.866, -1.4], [1.466, -0.266], [0.7, -1.1], [0, -2.933], [-0.8, 0]], 'v': [[90.8, -22.4], [75.4, -18.8], [77.65, -34.2], [79.8, -49], [83.7, -75.9], [83.8, -77.8], [76.8, -84.8], [71.6, -82.95], [69.3, -76.7], [62.75, -47.1], [52.55, -29.05], [41.5, -23.1], [35.2, -25.3], [33.4, -32.6], [34, -37.65], [35.8, -45.7], [38.65, -59.55], [39.6, -70.2], [36.15, -81.1], [26.6, -84.8], [2.7, -70.8], [-0.1, -63.8], [0.95, -60.75], [3.4, -59.4], [6.5, -61.3], [14.85, -70.05], [21.7, -72.9], [25.4, -68.1], [24.65, -60.8], [22.4, -49.8], [19.9, -37.75], [19.1, -29.6], [23.6, -16.05], [36.7, -10.8], [53, -16.9], [65, -35.4], [64, -29], [62, -14.9], [33.5, -0.4], [24.1, 18.3], [28.65, 28.65], [41.5, 32.7], [62.35, 23.25], [73.5, -5.9], [73.8, -8.3], [91.7, -12.1], [94.95, -14.15], [96, -18.2], [92.6, -22.6]], 'c': True}, 'ix': 2}, 'nm': 'Y', 'mn': 'ADBE Vector Shape - Group', 'hd': False}, {'ind': 1, 'ty': 'sh', 'ix': 2, 'ks': {'a': 0, 'k': {'i': [[0, 0], [9.266, 0], [1.166, 1.233], [0, 1.866], [-16.134, 5.6]], 'o': [[-2.334, 17.466], [-2.134, 0], [-1.167, -1.234], [0, -8], [0, 0]], 'v': [[60.4, -3.7], [43, 22.5], [38.05, 20.65], [36.3, 16], [60.5, -4.4]], 'c': True}, 'ix': 2}, 'nm': 'Y', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'Y', 'np': 5, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'F', 'size': 30, 'style': 'Regular', 'w': 71.2, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[1.866, 0.267], [11.333, 0], [8.5, -3.733], [0, -8.266], [-0.734, -2.066], [-0.8, -0.666], [-1.8, 0], [-1.334, 0.9], [0, 1.2], [0.4, 0.6], [0, 2.267], [-2.934, 1.667], [-7.2, 0.667], [0.8, -7.333], [1.866, 0], [1.066, -1.1], [0, -2.066], [-1.1, -0.866], [-1.534, 0], [0, 0], [0, 0], [2.566, -3.1], [3.8, 0], [3.2, 4.2], [0.766, 0.534], [0.8, 0], [0.766, -1.2], [0, -1.6], [-0.734, -1.133], [-3.8, -1.966], [-4.534, 0], [-4.567, 4.667], [-1.4, 11], [0, 0], [0, 0], [-1.334, 1.3], [0, 2.267], [0.833, 0.867], [2.466, 0], [0, 0], [-0.8, 9.867], [0, 0], [-3.9, -0.2], [-3.934, -0.333], [0, 0], [0, 4.6], [0.7, 0.867]], 'o': [[-8.667, -1.2], [-16.334, 0], [-8.5, 3.734], [0, 2.534], [0.733, 2.067], [1.266, 1.067], [1.666, 0], [1.333, -0.9], [0, -0.6], [-1.334, -2.066], [0, -3.266], [2.933, -1.666], [-0.934, 10.467], [-1.8, 0.067], [-2.067, 0], [-1.067, 1.1], [0, 1.6], [1.1, 0.867], [0, 0], [0, 0], [-0.734, 6.667], [-2.567, 3.1], [-4.734, 0], [-1.2, -1.533], [-0.767, -0.533], [-1.134, 0], [-0.767, 1.2], [0, 1.6], [1.8, 2.8], [3.8, 1.967], [8, 0], [4.566, -4.666], [0, 0], [0, 0], [2.466, 0], [1.333, -1.3], [0, -1.466], [-0.834, -0.866], [0, 0], [0.866, -8.133], [0, 0], [4.266, 0], [3.9, 0.2], [0, 0], [4.933, 0.334], [0, -1.4], [-0.7, -0.866]], 'v': [[88.7, -82.9], [58.7, -84.7], [21.45, -79.1], [8.7, -61.1], [9.8, -54.2], [12.1, -50.1], [16.7, -48.5], [21.2, -49.85], [23.2, -53], [22.6, -54.8], [20.6, -61.3], [25, -68.7], [40.2, -72.2], [37.6, -45.5], [32.1, -45.4], [27.4, -43.75], [25.8, -39], [27.45, -35.3], [31.4, -34], [36.2, -34], [35.6, -28.5], [30.65, -13.85], [21.1, -9.2], [9.2, -15.5], [6.25, -18.6], [3.9, -19.4], [1.05, -17.6], [-0.1, -13.4], [1, -9.3], [9.4, -2.15], [21.9, 0.8], [40.75, -6.2], [49.7, -29.7], [50.3, -34], [67.4, -34], [73.1, -35.95], [75.1, -41.3], [73.85, -44.8], [68.9, -46.1], [51.7, -45.8], [54.2, -72.8], [58.7, -72.8], [70.95, -72.5], [82.7, -71.7], [86.2, -71.4], [93.6, -77.8], [92.55, -81.2]], 'c': True}, 'ix': 2}, 'nm': 'F', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'F', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': ' ', 'size': 30, 'style': 'Regular', 'w': 26.5, 'data': {}, 'fFamily': 'Pacifico'}, {'ch': 'B', 'size': 30, 'style': 'Regular', 'w': 82.7, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[0, 5.667], [5.933, 4.067], [12.066, 0], [7.533, -1.8], [5.6, -3.2], [0.7, -1.2], [0, -1.666], [-0.634, -0.833], [-1.2, 0], [-2.134, 1.267], [-6.667, 1.834], [-7.134, 0], [-3.8, -2.233], [0, -3.866], [2.2, -2.3], [3.833, -1.266], [4.733, -0.133], [0.8, -1.2], [0, -1.933], [-0.534, -0.6], [-1.334, -0.066], [-2.5, -2], [0, -2.933], [4.366, -2.7], [9.333, 0], [3.2, 0.267], [-1.734, 8.9], [-1.734, 5.2], [0, 0.934], [4.066, 0], [1.4, -0.666], [0.466, -1.666], [1.733, -10.233], [0.6, -9.333], [-0.9, -1.067], [-2.4, 0], [-1.534, 0.933], [-0.067, 1.866], [-3.334, 0], [-6.334, 2.1], [-3.3, 3.867], [0, 5.267], [2.133, 2.567], [4.133, 1.134], [-4, 4.1]], 'o': [[0, -6.666], [-5.934, -4.066], [-7.867, 0], [-7.534, 1.8], [-2.667, 1.534], [-0.7, 1.2], [0, 1.267], [0.633, 0.834], [1.466, 0], [4.666, -2.8], [6.666, -1.833], [7.866, 0], [3.8, 2.234], [0, 3.067], [-2.2, 2.3], [-3.834, 1.267], [-2.134, 0.067], [-0.8, 1.2], [0, 1.334], [0.533, 0.6], [5.866, 0.2], [2.5, 2], [0, 4.2], [-4.367, 2.7], [-2, 0], [0.733, -8.066], [1.733, -8.9], [0.4, -1.2], [0, -2.266], [-2.267, 0], [-1.4, 0.667], [-2.667, 9.534], [-1.734, 10.234], [-0.134, 2.066], [0.9, 1.066], [2.4, 0], [1.533, -0.934], [2, 0.2], [8.933, 0], [6.333, -2.1], [3.3, -3.866], [0, -3.333], [-2.134, -2.566], [7.666, -1.8], [4, -4.1]], 'v': [[86.8, -64], [77.9, -80.1], [50.9, -86.2], [27.8, -83.5], [8.1, -76], [3.05, -71.9], [2, -67.6], [2.95, -64.45], [5.7, -63.2], [11.1, -65.1], [28.1, -72.05], [48.8, -74.8], [66.3, -71.45], [72, -62.3], [68.7, -54.25], [59.65, -48.9], [46.8, -46.8], [42.4, -44.9], [41.2, -40.2], [42, -37.3], [44.8, -36.3], [57.35, -33], [61.1, -25.6], [54.55, -15.25], [34, -11.2], [26.2, -11.6], [29.9, -37.05], [35.1, -58.2], [35.7, -61.4], [29.6, -64.8], [24.1, -63.8], [21.3, -60.3], [14.7, -30.65], [11.2, -1.3], [12.35, 3.4], [17.3, 5], [23.2, 3.6], [25.6, -0.6], [33.6, -0.3], [56.5, -3.45], [70.95, -12.4], [75.9, -26.1], [72.7, -34.95], [63.3, -40.5], [80.8, -49.35]], 'c': True}, 'ix': 2}, 'nm': 'B', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'B', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'U', 'size': 30, 'style': 'Regular', 'w': 89, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[-5.6, 0], [-5.1, 5.134], [-3.334, 9.8], [0, -2.533], [-2.934, -2.833], [-5.534, 0], [-3.4, 1.934], [-3.467, 4.2], [0, 2.6], [0.5, 0.8], [0.866, 0], [0.8, -0.933], [2.1, -1.466], [2.2, 0], [1.233, 1.434], [0, 2.734], [-0.534, 3.867], [-1.8, 10.2], [-0.434, 2.934], [0, 1.8], [1.133, 1.4], [2.333, 0], [0.9, -1.333], [0.466, -3.4], [3.5, -9.5], [4.1, -4.266], [4, 0], [1.2, 1.267], [0, 2.134], [-0.2, 1.367], [-0.334, 1.534], [-0.134, 0.6], [0, 0], [-0.467, 2.867], [0, 3.4], [2.3, 2.467], [4.066, 0], [6.8, -9.333], [0, -2.066], [-0.7, -0.9], [-0.934, 0], [-0.934, 1.267], [-2.667, 1.9], [-2, 0], [-0.634, -0.8], [0, -1.6], [0.5, -2.4], [0.133, -0.533], [0, 0], [0, -2.933], [-2.867, -3.1]], 'o': [[6.666, 0], [5.1, -5.133], [-1.067, 7.334], [0, 4.534], [2.933, 2.834], [3.733, 0], [3.4, -1.933], [1.266, -1.533], [0, -1.4], [-0.5, -0.8], [-1, 0], [-2.867, 3.4], [-2.1, 1.467], [-2.067, 0], [-1.234, -1.433], [0, -1.866], [1.066, -8.533], [0.866, -5.266], [0.433, -2.933], [0, -3.133], [-1.134, -1.4], [-2.6, 0], [-0.9, 1.334], [-1.934, 14.8], [-3.5, 9.5], [-4.1, 4.267], [-2.2, 0], [-1.2, -1.266], [0, -1.333], [0.2, -1.366], [0.333, -1.533], [0, 0], [1.133, -4.933], [0.466, -2.866], [0, -4.8], [-2.3, -2.466], [-9.134, 0], [-1.867, 2.6], [0, 1.134], [0.7, 0.9], [1.133, 0], [2.933, -3.933], [2.666, -1.9], [1.066, 0], [0.633, 0.8], [0, 2.8], [-0.5, 2.4], [0, 0], [-0.867, 4.2], [0, 5.2], [2.866, 3.1]], 'v': [[33.2, 0.5], [50.85, -7.2], [63.5, -29.6], [61.9, -14.8], [66.3, -3.75], [79, 0.5], [89.7, -2.4], [100, -11.6], [101.9, -17.8], [101.15, -21.1], [99.1, -22.3], [96.4, -20.9], [88.95, -13.6], [82.5, -11.4], [77.55, -13.55], [75.7, -19.8], [76.5, -28.4], [80.8, -56.5], [82.75, -68.8], [83.4, -75.9], [81.7, -82.7], [76.5, -84.8], [71.25, -82.8], [69.2, -75.7], [61.05, -39.25], [49.65, -18.6], [37.5, -12.2], [32.4, -14.1], [30.6, -19.2], [30.9, -23.25], [31.7, -27.6], [32.4, -30.8], [36.5, -49.1], [38.9, -60.8], [39.6, -70.2], [36.15, -81.1], [26.6, -84.8], [2.7, -70.8], [-0.1, -63.8], [0.95, -60.75], [3.4, -59.4], [6.5, -61.3], [14.9, -70.05], [21.9, -72.9], [24.45, -71.7], [25.4, -68.1], [24.65, -60.3], [23.7, -55.9], [17.5, -27.3], [16.2, -16.6], [20.5, -4.15]], 'c': True}, 'ix': 2}, 'nm': 'U', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'U', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'L', 'size': 30, 'style': 'Regular', 'w': 67.3, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[0.866, 0], [0.8, -0.933], [2.766, -1.3], [3.866, 0], [2, 0.4], [3.733, 0.934], [4.266, 0.734], [-0.334, 3.2], [0, 0], [-3.2, 3.834], [-5.867, 0], [-1.634, -1.633], [0, -2.8], [0.4, -1.866], [0, -0.6], [-1.067, -0.9], [-1.867, 0], [-1.467, 2.5], [0, 4.067], [3.866, 3.734], [7.2, 0], [3.933, -1.366], [3.066, -2.666], [2, -4.333], [0.4, -6.666], [0, 0], [0, 0], [3.133, -2.166], [0, -3.266], [-2.233, -1.7], [-3.734, 0], [-3.4, 6.2], [-3.8, -1.666], [-2.934, -0.866], [-3.467, 0], [-3.5, 1.8], [-3.734, 4.467], [0, 2.6], [0.5, 0.8]], 'o': [[-1, 0], [-2.467, 2.867], [-2.767, 1.3], [-1.534, 0], [-2, -0.4], [-6.4, -1.6], [0.533, -2.333], [0, 0], [0.866, -8.2], [3.2, -3.833], [3.333, 0], [1.633, 1.634], [0, 1.467], [-0.267, 1.6], [0, 1.667], [1.066, 0.9], [2.6, 0], [1.466, -2.5], [0, -6], [-3.867, -3.733], [-4.4, 0], [-3.934, 1.367], [-3.534, 3.067], [-2, 4.334], [0, 0], [0, 0], [-5.2, 0], [-3.133, 2.167], [0, 2.667], [2.233, 1.7], [6.8, 0], [3.533, 1.067], [4.2, 1.734], [2.933, 0.866], [4.933, 0], [3.5, -1.8], [1.266, -1.533], [0, -1.4], [-0.5, -0.8]], 'v': [[77.4, -22.3], [74.7, -20.9], [66.85, -14.65], [56.9, -12.7], [51.6, -13.3], [43, -15.3], [27, -18.8], [28.3, -27.1], [30.6, -49.8], [36.7, -67.85], [50.3, -73.6], [57.75, -71.15], [60.2, -64.5], [59.6, -59.5], [59.2, -56.2], [60.8, -52.35], [65.2, -51], [71.3, -54.75], [73.5, -64.6], [67.7, -79.2], [51.1, -84.8], [38.6, -82.75], [28.1, -76.7], [19.8, -65.6], [16.2, -49.1], [14.4, -20], [13.1, -20], [0.6, -16.75], [-4.1, -8.6], [-0.75, -2.05], [8.2, 0.5], [23.5, -8.8], [34.5, -4.7], [45.2, -0.8], [54.8, 0.5], [67.45, -2.2], [78.3, -11.6], [80.2, -17.8], [79.45, -21.1]], 'c': True}, 'ix': 2}, 'nm': 'L', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'L', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'N', 'size': 30, 'style': 'Regular', 'w': 88.4, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[-2.467, 0], [-0.9, 1.334], [-0.467, 3.4], [-3.4, 9.5], [-4, 4.267], [-4, 0], [-1.2, -1.266], [0, -2.133], [0.2, -1.366], [0.333, -1.533], [0.133, -0.6], [0, 0], [0.366, -2.6], [0, -2.2], [-3.2, -3.366], [-5.667, 0], [-3.4, 1.934], [-3.467, 4.2], [0, 2.6], [0.5, 0.8], [0.866, 0], [0.8, -0.933], [2.1, -1.466], [2.2, 0], [1.3, 1.4], [0, 2.8], [-0.667, 3.334], [0, 0], [0, 2.934], [2.766, 3.1], [5.466, 0], [5.133, -5.1], [3.333, -9.866], [0, 3.867], [1.833, 2.267], [3.666, 0], [4, -2.433], [3.266, -4.466], [0.4, -1.033], [0, -1.133], [-0.7, -0.9], [-0.934, 0], [-0.934, 1.267], [-2.5, 1.767], [-1.667, 0], [0, -3], [0.666, -5.333], [0.933, -5.7], [0.133, -0.8], [0.4, -2.933], [0, -2.066], [-1.067, -1.1]], 'o': [[2.6, 0], [0.9, -1.333], [1.933, -14.8], [3.4, -9.5], [4, -4.266], [2.2, 0], [1.2, 1.267], [0, 1.334], [-0.2, 1.367], [-0.334, 1.534], [0, 0], [-0.867, 4], [-0.367, 2.6], [0, 5.667], [3.2, 3.367], [3.733, 0], [3.4, -1.933], [1.266, -1.533], [0, -1.4], [-0.5, -0.8], [-1, 0], [-2.867, 3.4], [-2.1, 1.467], [-2.334, 0], [-1.3, -1.4], [0, -2.4], [0, 0], [0.866, -4.2], [0, -5.2], [-2.767, -3.1], [-6.934, 0], [-5.134, 5.1], [1.066, -7.333], [0, -4.333], [-1.834, -2.266], [-4.4, 0], [-4, 2.434], [-1.067, 1.467], [-0.4, 1.034], [0, 1.134], [0.7, 0.9], [1.133, 0], [2.866, -3.866], [2.5, -1.766], [2.2, 0], [0, 2.667], [-0.734, 6.267], [-0.934, 5.7], [-1, 5.934], [-0.4, 2.934], [0, 3.067], [1.066, 1.1]], 'v': [[23.2, 0.5], [28.45, -1.5], [30.5, -8.6], [38.5, -45.05], [49.6, -65.7], [61.6, -72.1], [66.7, -70.2], [68.5, -65.1], [68.2, -61.05], [67.4, -56.7], [66.7, -53.5], [62.7, -35.2], [60.85, -25.3], [60.3, -18.1], [65.1, -4.55], [78.4, 0.5], [89.1, -2.4], [99.4, -11.6], [101.3, -17.8], [100.55, -21.1], [98.5, -22.3], [95.8, -20.9], [88.35, -13.6], [81.9, -11.4], [76.45, -13.5], [74.5, -19.8], [75.5, -28.4], [81.6, -57], [82.9, -67.7], [78.75, -80.15], [66.4, -84.8], [48.3, -77.15], [35.6, -54.7], [37.2, -71.5], [34.45, -81.4], [26.2, -84.8], [13.6, -81.15], [2.7, -70.8], [0.5, -67.05], [-0.1, -63.8], [0.95, -60.75], [3.4, -59.4], [6.5, -61.3], [14.55, -69.75], [20.8, -72.4], [24.1, -67.9], [23.1, -55.9], [20.6, -37.95], [19, -28.2], [16.9, -14.9], [16.3, -7.4], [17.9, -1.15]], 'c': True}, 'ix': 2}, 'nm': 'N', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'N', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'M', 'size': 30, 'style': 'Regular', 'w': 123.2, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[-2.467, 0], [-0.9, 1.334], [-0.467, 3.4], [-3.3, 9.434], [-3.467, 3.7], [-3.267, 0], [-0.967, -1.2], [0, -2.533], [3.066, -16.133], [0.733, -4.433], [0, -2.733], [-1.034, -1.066], [-2.267, 0], [-1.167, 1.367], [-0.467, 4], [-3.1, 9.334], [-3.434, 4.034], [-3.134, 0], [-0.9, -1.166], [0, -2.333], [0.2, -1.366], [0.333, -1.533], [0.133, -0.6], [0, 0], [0, -3.933], [-3.2, -3.366], [-5.667, 0], [-3.4, 1.934], [-3.467, 4.2], [0, 2.6], [0.5, 0.8], [0.866, 0], [0.8, -0.933], [2.1, -1.466], [2.2, 0], [1.3, 1.4], [0, 2.8], [-0.667, 3.334], [0, 0], [0, 2.934], [2.5, 3], [4.666, 0], [4.466, -4], [3.333, -9.2], [0, 2.2], [2.5, 3.067], [4.333, 0], [4.733, -4.3], [3.8, -10.866], [-0.267, 1.534], [-0.334, 2.434], [0, 1.8], [1.966, 2.334], [3.666, 0], [3.933, -2.433], [3.2, -4.466], [0.433, -1.1], [0, -1.066], [-0.7, -0.9], [-0.934, 0], [-0.934, 1.267], [-2.434, 1.767], [-1.734, 0], [0, -3], [0.6, -4.8], [1.733, -10.466], [0.433, -3.233], [0, -2.066], [-1.067, -1.1]], 'o': [[2.6, 0], [0.9, -1.333], [2.2, -16.066], [3.3, -9.433], [3.466, -3.7], [1.933, 0], [0.966, 1.2], [0, 4.667], [-1.134, 6], [-0.734, 4.434], [0, 2.934], [1.033, 1.067], [2.6, 0], [1.166, -1.366], [1.933, -14.933], [3.1, -9.333], [3.433, -4.033], [1.666, 0], [0.9, 1.167], [0, 1.334], [-0.2, 1.367], [-0.334, 1.534], [0, 0], [-1.6, 7.467], [0, 5.667], [3.2, 3.367], [3.733, 0], [3.4, -1.933], [1.266, -1.533], [0, -1.4], [-0.5, -0.8], [-1, 0], [-2.867, 3.4], [-2.1, 1.467], [-2.334, 0], [-1.3, -1.4], [0, -2.4], [0, 0], [0.866, -4.2], [0, -5.4], [-2.5, -3], [-5.8, 0], [-4.467, 4], [0.6, -3.266], [0, -5.6], [-2.5, -3.066], [-5.667, 0], [-4.734, 4.3], [0.133, -0.6], [0.266, -1.533], [0.333, -2.433], [0, -4.466], [-1.967, -2.333], [-3.934, 0], [-3.934, 2.434], [-1, 1.4], [-0.434, 1.1], [0, 1.134], [0.7, 0.9], [1.133, 0], [2.933, -3.866], [2.433, -1.766], [2.2, 0], [0, 3.2], [-1, 7.667], [-1, 5.667], [-0.434, 3.234], [0, 3.067], [1.066, 1.1]], 'v': [[23.2, 0.5], [28.45, -1.5], [30.5, -8.6], [38.75, -46.85], [48.9, -66.55], [59, -72.1], [63.35, -70.3], [64.8, -64.7], [60.2, -33.5], [57.4, -17.85], [56.3, -7.1], [57.85, -1.1], [62.8, 0.5], [68.45, -1.55], [70.9, -9.6], [78.45, -46], [88.25, -66.05], [98.1, -72.1], [101.95, -70.35], [103.3, -65.1], [103, -61.05], [102.2, -56.7], [101.5, -53.5], [97.5, -35.2], [95.1, -18.1], [99.9, -4.55], [113.2, 0.5], [123.9, -2.4], [134.2, -11.6], [136.1, -17.8], [135.35, -21.1], [133.3, -22.3], [130.6, -20.9], [123.15, -13.6], [116.7, -11.4], [111.25, -13.5], [109.3, -19.8], [110.3, -28.4], [116.4, -57], [117.7, -67.7], [113.95, -80.3], [103.2, -84.8], [87.8, -78.8], [76.1, -59], [77, -67.2], [73.25, -80.2], [63, -84.8], [47.4, -78.35], [34.6, -55.6], [35.2, -58.8], [36.1, -64.75], [36.6, -71.1], [33.65, -81.3], [25.2, -84.8], [13.4, -81.15], [2.7, -70.8], [0.55, -67.05], [-0.1, -63.8], [0.95, -60.75], [3.4, -59.4], [6.5, -61.3], [14.55, -69.75], [20.8, -72.4], [24.1, -67.9], [23.2, -55.9], [19.1, -28.7], [16.95, -15.35], [16.3, -7.4], [17.9, -1.15]], 'c': True}, 'ix': 2}, 'nm': 'M', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'M', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'D', 'size': 30, 'style': 'Regular', 'w': 83.6, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[-3.867, 0], [-7.667, 4.134], [-4, 7.5], [0, 10.067], [3.2, 5.467], [5.933, 2.834], [8.133, 0], [6.2, -1.633], [4.6, -3.133], [0.533, -1.033], [0, -1.6], [-0.667, -0.966], [-1.134, 0], [-0.867, 0.6], [-5.234, 1.667], [-5.334, 0], [-4.534, -4.333], [0, -7.933], [5.766, -7.066], [11.666, 0], [2, 0.2], [-1.734, 8.967], [-1.734, 5.334], [0, 0.934], [4.066, 0], [1.4, -0.666], [0.466, -1.666], [1.733, -9.7], [0.466, -6.6], [-1, -1.066], [-2.667, -0.333]], 'o': [[10.6, 0], [7.666, -4.133], [4, -7.5], [0, -7.733], [-3.2, -5.466], [-5.934, -2.833], [-5.734, 0], [-6.2, 1.634], [-1.267, 0.867], [-0.534, 1.034], [0, 1.4], [0.666, 0.967], [1, 0], [4.2, -2.733], [5.233, -1.666], [8.266, 0], [4.533, 4.334], [0, 11.8], [-5.767, 7.067], [-2.534, 0], [0.733, -8.133], [1.733, -8.966], [0.4, -1.2], [0, -2.266], [-2.267, 0], [-1.4, 0.667], [-2.467, 9], [-1.734, 9.7], [-0.134, 2.4], [1, 1.067], [4.866, 0.666]], 'v': [[30.8, 0.5], [58.2, -5.7], [75.7, -23.15], [81.7, -49.5], [76.9, -69.3], [63.2, -81.75], [42.1, -86], [24.2, -83.55], [8, -76.4], [5.3, -73.55], [4.5, -69.6], [5.5, -66.05], [8.2, -64.6], [11, -65.5], [25.15, -72.1], [41, -74.6], [60.2, -68.1], [67, -49.7], [58.35, -21.4], [32.2, -10.8], [25.4, -11.1], [29.1, -36.75], [34.3, -58.2], [34.9, -61.4], [28.8, -64.8], [23.3, -63.8], [20.5, -60.3], [14.2, -32.25], [10.9, -7.8], [12.2, -2.6], [17.7, -0.5]], 'c': True}, 'ix': 2}, 'nm': 'D', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'D', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}, {'ch': 'I', 'size': 30, 'style': 'Regular', 'w': 49.5, 'data': {'shapes': [{'ty': 'gr', 'it': [{'ind': 0, 'ty': 'sh', 'ix': 1, 'ks': {'a': 0, 'k': {'i': [[1.733, 0], [0, 0], [3.066, -0.133], [0, -4.533], [-0.9, -0.766], [-2.4, 0], [0, 0], [1.333, -7.733], [0, 0], [1.6, -10.666], [0, 0], [0, 0], [2.133, -1.333], [0, -2.4], [-1, -0.8], [-1.467, 0], [-2.2, 0.333], [-4.2, 0], [-3.334, -0.134], [-1.667, 0], [-1.367, 1.2], [0, 1.734], [1.266, 0.934], [3.533, 0], [1.4, -0.066], [-1.467, 9.8], [0, 0], [-1.2, 7.134], [-0.134, 0.8], [-3.867, 0], [-1.334, 1.3], [0, 2.134], [1.2, 0.834]], 'o': [[0, 0], [-4.4, 0], [-6.534, 0.334], [0, 1.4], [0.9, 0.767], [0, 0], [-1.067, 8.2], [0, 0], [-0.734, 4.4], [0, 0], [0, 0], [-3.867, 0.067], [-2.133, 1.334], [0, 1.534], [1, 0.8], [0.933, 0], [5, -0.734], [1.066, 0], [3.6, 0.133], [2.466, 0], [1.366, -1.2], [0, -1.866], [-1.267, -0.933], [-2.4, 0], [0.866, -6.6], [0, 0], [0.266, -1.6], [1.066, -6.4], [2, -0.066], [2.466, 0], [1.333, -1.3], [0, -1.2], [-1.2, -0.833]], 'v': [[49.4, -84.2], [31.1, -84.3], [19.9, -84.1], [10.1, -76.8], [11.45, -73.55], [16.4, -72.4], [24.8, -72.5], [21.2, -48.6], [19, -35.5], [15.5, -12.9], [15.2, -10.7], [10.5, -10.6], [1.5, -8.5], [-1.7, -2.9], [-0.2, 0.6], [3.5, 1.8], [8.2, 1.3], [22, 0.2], [28.6, 0.4], [36.5, 0.6], [42.25, -1.2], [44.3, -5.6], [42.4, -9.8], [35.2, -11.2], [29.5, -11.1], [33, -35.7], [35.1, -48.8], [37.3, -61.9], [39.1, -72.7], [47.9, -72.8], [53.6, -74.75], [55.6, -79.9], [53.8, -82.95]], 'c': True}, 'ix': 2}, 'nm': 'I', 'mn': 'ADBE Vector Shape - Group', 'hd': False}], 'nm': 'I', 'np': 3, 'cix': 2, 'bm': 0, 'ix': 1, 'mn': 'ADBE Vector Group', 'hd': False}]}, 'fFamily': 'Pacifico'}]</t>
   </si>
 </sst>
 </file>
@@ -389,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,38 +450,82 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>29.9700012207031</v>
       </c>
       <c r="C2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>900.000036657751</v>
+      </c>
+      <c r="E2">
+        <v>1920</v>
+      </c>
+      <c r="F2">
+        <v>1080</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>